<commit_message>
research and database update
</commit_message>
<xml_diff>
--- a/docs/watering_tracking_database.xlsx
+++ b/docs/watering_tracking_database.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28914"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xing2\Documents\GitHub\automated_crop_watering_system_project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB8F8A7-0A3A-4A38-8614-902755F68B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{02A80973-50CA-410A-A377-8DBCB3D9A580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{526E19EB-3246-4824-ACE4-8785D31DA4D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracking" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="7">
-  <si>
-    <t>average</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
   <si>
     <t>Time</t>
   </si>
@@ -47,7 +44,7 @@
     <t>Wetness (%)</t>
   </si>
   <si>
-    <t>No</t>
+    <t>average</t>
   </si>
   <si>
     <t>Watering Log</t>
@@ -58,6 +55,24 @@
   <si>
     <t>Hand</t>
   </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Tempterature</t>
+  </si>
+  <si>
+    <t>Humidity</t>
+  </si>
+  <si>
+    <t>11 C</t>
+  </si>
+  <si>
+    <t>Weather</t>
+  </si>
+  <si>
+    <t>Cloudy, with partial showers</t>
+  </si>
 </sst>
 </file>
 
@@ -66,7 +81,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,7 +135,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -270,6 +285,66 @@
       </top>
       <bottom style="medium">
         <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -278,7 +353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -287,21 +362,37 @@
     <xf numFmtId="9" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,17 +728,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802438E6-19C0-483A-A8DC-08A8C4B3AED7}">
-  <dimension ref="A1:S42"/>
+  <dimension ref="A1:S48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47:C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -658,102 +750,102 @@
     <col min="19" max="19" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="8">
+    <row r="1" spans="2:19" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:19">
+      <c r="B2" s="13">
         <v>45797</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="8">
+      <c r="C2" s="14"/>
+      <c r="D2" s="13">
         <v>45798</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="8">
+      <c r="E2" s="14"/>
+      <c r="F2" s="13">
         <v>45799</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="8">
+      <c r="G2" s="14"/>
+      <c r="H2" s="13">
         <v>45800</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="8">
+      <c r="I2" s="14"/>
+      <c r="J2" s="13">
         <v>45801</v>
       </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="8">
+      <c r="K2" s="14"/>
+      <c r="L2" s="13">
         <v>45802</v>
       </c>
-      <c r="M2" s="9"/>
-      <c r="N2" s="8">
+      <c r="M2" s="14"/>
+      <c r="N2" s="13">
         <v>45803</v>
       </c>
-      <c r="O2" s="9"/>
-      <c r="P2" s="8">
+      <c r="O2" s="14"/>
+      <c r="P2" s="13">
         <v>45804</v>
       </c>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="8">
+      <c r="Q2" s="14"/>
+      <c r="R2" s="13">
         <v>45805</v>
       </c>
-      <c r="S2" s="9"/>
-    </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S2" s="14"/>
+    </row>
+    <row r="3" spans="2:19">
       <c r="B3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>2</v>
-      </c>
       <c r="D3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>2</v>
-      </c>
       <c r="F3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>2</v>
-      </c>
       <c r="H3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>2</v>
-      </c>
       <c r="J3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="7" t="s">
-        <v>2</v>
-      </c>
       <c r="L3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="7" t="s">
-        <v>2</v>
-      </c>
       <c r="N3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="7" t="s">
-        <v>2</v>
-      </c>
       <c r="P3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="Q3" s="7" t="s">
-        <v>2</v>
-      </c>
       <c r="R3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:19">
       <c r="B4" s="2">
         <v>0.90372685185185186</v>
       </c>
@@ -763,11 +855,11 @@
       <c r="D4" s="1">
         <v>4.8304398148148149E-4</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="8">
         <v>0.74</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19">
       <c r="B5" s="2">
         <v>0.90581327546296309</v>
       </c>
@@ -777,11 +869,11 @@
       <c r="D5" s="1">
         <v>1.0912766203703704E-2</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="8">
         <v>0.76</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19">
       <c r="B6" s="2">
         <v>0.90789936342592603</v>
       </c>
@@ -791,11 +883,11 @@
       <c r="D6" s="1">
         <v>2.1342974537037037E-2</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="8">
         <v>0.74</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19">
       <c r="B7" s="2">
         <v>0.90998508101851849</v>
       </c>
@@ -805,11 +897,11 @@
       <c r="D7" s="1">
         <v>3.1772881944444449E-2</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="8">
         <v>0.73</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19">
       <c r="B8" s="2">
         <v>0.91207133101851856</v>
       </c>
@@ -819,11 +911,11 @@
       <c r="D8" s="1">
         <v>4.2202766203703702E-2</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="8">
         <v>0.74</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19">
       <c r="B9" s="2">
         <v>0.91415709490740737</v>
       </c>
@@ -833,11 +925,11 @@
       <c r="D9" s="1">
         <v>5.2632812500000001E-2</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="8">
         <v>0.73</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19">
       <c r="B10" s="2">
         <v>0.91624322916666656</v>
       </c>
@@ -847,11 +939,11 @@
       <c r="D10" s="1">
         <v>6.3062638888888883E-2</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="8">
         <v>0.78</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:19">
       <c r="B11" s="2">
         <v>0.91832944444444453</v>
       </c>
@@ -861,11 +953,11 @@
       <c r="D11" s="1">
         <v>7.3492592592592595E-2</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="8">
         <v>0.78</v>
       </c>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:19">
       <c r="B12" s="2">
         <v>0.92041519675925931</v>
       </c>
@@ -873,18 +965,18 @@
         <v>0.78</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="10"/>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="2:19">
       <c r="B13" s="2">
         <v>0.92250140046296292</v>
       </c>
       <c r="C13" s="3">
         <v>0.78</v>
       </c>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="2:19">
       <c r="B14" s="2">
         <v>0.92458736111111106</v>
       </c>
@@ -892,45 +984,45 @@
         <v>0.76</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="10"/>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="2:19">
       <c r="B15" s="2">
         <v>0.92667320601851855</v>
       </c>
       <c r="C15" s="3">
         <v>0.79</v>
       </c>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="2:19">
       <c r="B16" s="2">
         <v>0.92875912037037034</v>
       </c>
       <c r="C16" s="3">
         <v>0.78</v>
       </c>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5">
       <c r="B17" s="2">
         <v>0.93084533564814809</v>
       </c>
       <c r="C17" s="3">
         <v>0.77</v>
       </c>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5">
       <c r="B18" s="2">
         <v>0.93293137731481479</v>
       </c>
       <c r="C18" s="3">
         <v>0.74</v>
       </c>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5">
       <c r="B19" s="2">
         <v>0.9350171990740741</v>
       </c>
@@ -938,9 +1030,9 @@
         <v>0.77</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5">
       <c r="B20" s="2">
         <v>0.937103113425926</v>
       </c>
@@ -948,9 +1040,9 @@
         <v>0.7</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" spans="1:5">
       <c r="B21" s="2">
         <v>0.9391891550925926</v>
       </c>
@@ -958,9 +1050,9 @@
         <v>0.77</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="10"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:5">
       <c r="B22" s="2">
         <v>0.94127504629629632</v>
       </c>
@@ -968,9 +1060,9 @@
         <v>0.78</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:5">
       <c r="B23" s="2">
         <v>0.94336109953703706</v>
       </c>
@@ -978,9 +1070,9 @@
         <v>0.76</v>
       </c>
       <c r="D23" s="1"/>
-      <c r="E23" s="10"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:5">
       <c r="B24" s="2">
         <v>0.94544737268518531</v>
       </c>
@@ -988,9 +1080,9 @@
         <v>0.78</v>
       </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="10"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="1:5">
       <c r="B25" s="2">
         <v>0.94753321759259257</v>
       </c>
@@ -998,9 +1090,9 @@
         <v>0.75</v>
       </c>
       <c r="D25" s="1"/>
-      <c r="E25" s="10"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:5">
       <c r="B26" s="2">
         <v>0.94833349537037037</v>
       </c>
@@ -1008,9 +1100,9 @@
         <v>0.74</v>
       </c>
       <c r="D26" s="1"/>
-      <c r="E26" s="10"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="1:5">
       <c r="B27" s="2">
         <v>0.95876315972222226</v>
       </c>
@@ -1018,9 +1110,9 @@
         <v>0.74</v>
       </c>
       <c r="D27" s="1"/>
-      <c r="E27" s="10"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:5">
       <c r="B28" s="2">
         <v>0.96919327546296297</v>
       </c>
@@ -1028,9 +1120,9 @@
         <v>0.75</v>
       </c>
       <c r="D28" s="1"/>
-      <c r="E28" s="10"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:5">
       <c r="B29" s="2">
         <v>0.97962309027777772</v>
       </c>
@@ -1038,9 +1130,9 @@
         <v>0.77</v>
       </c>
       <c r="D29" s="1"/>
-      <c r="E29" s="10"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:5">
       <c r="B30" s="2">
         <v>0.99005290509259258</v>
       </c>
@@ -1048,9 +1140,9 @@
         <v>0.75</v>
       </c>
       <c r="D30" s="1"/>
-      <c r="E30" s="10"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="8"/>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="1"/>
       <c r="B31" s="2">
         <v>4.8304398148148149E-4</v>
@@ -1059,58 +1151,88 @@
         <v>0.74</v>
       </c>
       <c r="D31" s="1"/>
-      <c r="E31" s="10"/>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1">
       <c r="B32" s="4" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C32" s="5">
         <f>AVERAGE(C4:C31)</f>
         <v>0.76249999999999984</v>
       </c>
       <c r="D32" s="1"/>
-      <c r="E32" s="10"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="1"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" s="1"/>
     </row>
-    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="39" spans="1:3">
       <c r="B39" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="12"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="B40" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="12"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="6" t="s">
+      <c r="C40" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="7" t="s">
+    </row>
+    <row r="41" spans="1:3">
+      <c r="B41" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="6" t="s">
-        <v>3</v>
-      </c>
       <c r="C41" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B42" s="9">
         <v>0</v>
       </c>
-      <c r="C42" s="14">
+      <c r="C42" s="10">
         <v>0</v>
       </c>
     </row>
+    <row r="44" spans="1:3">
+      <c r="B44" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="B45" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="22">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="B47" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="16"/>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="B48" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="18"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="P2:Q2"/>

</xml_diff>

<commit_message>
excel and code update
</commit_message>
<xml_diff>
--- a/docs/watering_tracking_database.xlsx
+++ b/docs/watering_tracking_database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xing2\Documents\GitHub\automated_crop_watering_system_project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274498DF-9A8C-4C2D-AF2A-2EE5DCF00C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1014A3BC-824F-49C2-8099-DB8310BCB1B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15345" xr2:uid="{526E19EB-3246-4824-ACE4-8785D31DA4D1}"/>
+    <workbookView xWindow="-16320" yWindow="6825" windowWidth="16410" windowHeight="15345" xr2:uid="{526E19EB-3246-4824-ACE4-8785D31DA4D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracking" sheetId="1" r:id="rId1"/>
@@ -761,10 +761,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -785,37 +798,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1153,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802438E6-19C0-483A-A8DC-08A8C4B3AED7}">
   <dimension ref="A1:AI104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,74 +1198,74 @@
   <sheetData>
     <row r="1" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B2" s="40">
+      <c r="B2" s="53">
         <v>45797</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="40">
+      <c r="C2" s="55"/>
+      <c r="D2" s="53">
         <v>45798</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="40">
+      <c r="E2" s="55"/>
+      <c r="F2" s="53">
         <v>45799</v>
       </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="40">
+      <c r="G2" s="55"/>
+      <c r="H2" s="53">
         <v>45800</v>
       </c>
-      <c r="I2" s="41"/>
-      <c r="J2" s="40">
+      <c r="I2" s="54"/>
+      <c r="J2" s="53">
         <v>45801</v>
       </c>
-      <c r="K2" s="41"/>
-      <c r="L2" s="40">
+      <c r="K2" s="54"/>
+      <c r="L2" s="53">
         <v>45802</v>
       </c>
-      <c r="M2" s="41"/>
-      <c r="N2" s="40">
+      <c r="M2" s="54"/>
+      <c r="N2" s="53">
         <v>45803</v>
       </c>
-      <c r="O2" s="41"/>
-      <c r="P2" s="40">
+      <c r="O2" s="54"/>
+      <c r="P2" s="53">
         <v>45804</v>
       </c>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="40">
+      <c r="Q2" s="54"/>
+      <c r="R2" s="53">
         <v>45805</v>
       </c>
-      <c r="S2" s="41"/>
-      <c r="T2" s="40">
+      <c r="S2" s="54"/>
+      <c r="T2" s="53">
         <v>45806</v>
       </c>
-      <c r="U2" s="41"/>
-      <c r="V2" s="40">
+      <c r="U2" s="54"/>
+      <c r="V2" s="53">
         <v>45807</v>
       </c>
-      <c r="W2" s="41"/>
-      <c r="X2" s="40">
+      <c r="W2" s="54"/>
+      <c r="X2" s="53">
         <v>45808</v>
       </c>
-      <c r="Y2" s="41"/>
-      <c r="Z2" s="40">
+      <c r="Y2" s="54"/>
+      <c r="Z2" s="53">
         <v>45809</v>
       </c>
-      <c r="AA2" s="41"/>
-      <c r="AB2" s="40">
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="53">
         <v>45810</v>
       </c>
-      <c r="AC2" s="41"/>
-      <c r="AD2" s="40">
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="53">
         <v>45811</v>
       </c>
-      <c r="AE2" s="41"/>
-      <c r="AF2" s="40">
+      <c r="AE2" s="54"/>
+      <c r="AF2" s="53">
         <v>45812</v>
       </c>
-      <c r="AG2" s="41"/>
-      <c r="AH2" s="40">
+      <c r="AG2" s="54"/>
+      <c r="AH2" s="53">
         <v>45813</v>
       </c>
-      <c r="AI2" s="41"/>
+      <c r="AI2" s="54"/>
     </row>
     <row r="3" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -1396,8 +1396,12 @@
       <c r="I4" s="19">
         <v>0.77</v>
       </c>
-      <c r="J4" s="37"/>
-      <c r="K4" s="36"/>
+      <c r="J4" s="17">
+        <v>4.3824618055555556E-2</v>
+      </c>
+      <c r="K4" s="19">
+        <v>0.75</v>
+      </c>
       <c r="L4" s="37"/>
       <c r="M4" s="36"/>
       <c r="N4" s="37"/>
@@ -1448,8 +1452,12 @@
       <c r="I5" s="19">
         <v>0.81</v>
       </c>
-      <c r="J5" s="37"/>
-      <c r="K5" s="36"/>
+      <c r="J5" s="17">
+        <v>8.5543750000000002E-2</v>
+      </c>
+      <c r="K5" s="19">
+        <v>0.76</v>
+      </c>
       <c r="L5" s="37"/>
       <c r="M5" s="36"/>
       <c r="N5" s="37"/>
@@ -1500,8 +1508,12 @@
       <c r="I6" s="19">
         <v>0.81</v>
       </c>
-      <c r="J6" s="37"/>
-      <c r="K6" s="36"/>
+      <c r="J6" s="17">
+        <v>0.12726281249999999</v>
+      </c>
+      <c r="K6" s="19">
+        <v>0.73</v>
+      </c>
       <c r="L6" s="37"/>
       <c r="M6" s="36"/>
       <c r="N6" s="37"/>
@@ -1552,8 +1564,12 @@
       <c r="I7" s="19">
         <v>0.76</v>
       </c>
-      <c r="J7" s="37"/>
-      <c r="K7" s="36"/>
+      <c r="J7" s="17">
+        <v>0.16898188657407406</v>
+      </c>
+      <c r="K7" s="19">
+        <v>0.73</v>
+      </c>
       <c r="L7" s="37"/>
       <c r="M7" s="36"/>
       <c r="N7" s="37"/>
@@ -1604,8 +1620,12 @@
       <c r="I8" s="19">
         <v>0.81</v>
       </c>
-      <c r="J8" s="37"/>
-      <c r="K8" s="36"/>
+      <c r="J8" s="17">
+        <v>0.21070064814814815</v>
+      </c>
+      <c r="K8" s="19">
+        <v>0.72</v>
+      </c>
       <c r="L8" s="37"/>
       <c r="M8" s="36"/>
       <c r="N8" s="37"/>
@@ -1656,8 +1676,12 @@
       <c r="I9" s="19">
         <v>0.78</v>
       </c>
-      <c r="J9" s="37"/>
-      <c r="K9" s="36"/>
+      <c r="J9" s="17">
+        <v>0.25241973379629629</v>
+      </c>
+      <c r="K9" s="19">
+        <v>0.73</v>
+      </c>
       <c r="L9" s="37"/>
       <c r="M9" s="36"/>
       <c r="N9" s="37"/>
@@ -1708,8 +1732,12 @@
       <c r="I10" s="19">
         <v>0.78</v>
       </c>
-      <c r="J10" s="37"/>
-      <c r="K10" s="36"/>
+      <c r="J10" s="17">
+        <v>0.29413939814814816</v>
+      </c>
+      <c r="K10" s="19">
+        <v>0.76</v>
+      </c>
       <c r="L10" s="37"/>
       <c r="M10" s="36"/>
       <c r="N10" s="37"/>
@@ -1760,8 +1788,12 @@
       <c r="I11" s="19">
         <v>0.76</v>
       </c>
-      <c r="J11" s="37"/>
-      <c r="K11" s="36"/>
+      <c r="J11" s="17">
+        <v>0.33586030092592595</v>
+      </c>
+      <c r="K11" s="19">
+        <v>0.73</v>
+      </c>
       <c r="L11" s="37"/>
       <c r="M11" s="36"/>
       <c r="N11" s="37"/>
@@ -1812,8 +1844,12 @@
       <c r="I12" s="19">
         <v>0.76</v>
       </c>
-      <c r="J12" s="37"/>
-      <c r="K12" s="36"/>
+      <c r="J12" s="17">
+        <v>0.37758187500000001</v>
+      </c>
+      <c r="K12" s="19">
+        <v>0.73</v>
+      </c>
       <c r="L12" s="37"/>
       <c r="M12" s="36"/>
       <c r="N12" s="37"/>
@@ -1864,8 +1900,12 @@
       <c r="I13" s="19">
         <v>0.76</v>
       </c>
-      <c r="J13" s="37"/>
-      <c r="K13" s="36"/>
+      <c r="J13" s="17">
+        <v>0.41930336805555557</v>
+      </c>
+      <c r="K13" s="19">
+        <v>0.75</v>
+      </c>
       <c r="L13" s="37"/>
       <c r="M13" s="36"/>
       <c r="N13" s="37"/>
@@ -1916,8 +1956,12 @@
       <c r="I14" s="19">
         <v>0.78</v>
       </c>
-      <c r="J14" s="37"/>
-      <c r="K14" s="36"/>
+      <c r="J14" s="17">
+        <v>0.46102739583333335</v>
+      </c>
+      <c r="K14" s="19">
+        <v>0.73</v>
+      </c>
       <c r="L14" s="37"/>
       <c r="M14" s="36"/>
       <c r="N14" s="37"/>
@@ -1968,8 +2012,12 @@
       <c r="I15" s="19">
         <v>0.77</v>
       </c>
-      <c r="J15" s="37"/>
-      <c r="K15" s="36"/>
+      <c r="J15" s="17">
+        <v>0.50275090277777779</v>
+      </c>
+      <c r="K15" s="19">
+        <v>0.71</v>
+      </c>
       <c r="L15" s="37"/>
       <c r="M15" s="36"/>
       <c r="N15" s="37"/>
@@ -2021,8 +2069,12 @@
       <c r="I16" s="19">
         <v>0.82</v>
       </c>
-      <c r="J16" s="37"/>
-      <c r="K16" s="36"/>
+      <c r="J16" s="17">
+        <v>0.54447665509259258</v>
+      </c>
+      <c r="K16" s="19">
+        <v>0.7</v>
+      </c>
       <c r="L16" s="37"/>
       <c r="M16" s="36"/>
       <c r="N16" s="37"/>
@@ -2067,8 +2119,12 @@
       <c r="I17" s="19">
         <v>0.81</v>
       </c>
-      <c r="J17" s="37"/>
-      <c r="K17" s="36"/>
+      <c r="J17" s="17">
+        <v>0.58620266203703708</v>
+      </c>
+      <c r="K17" s="19">
+        <v>0.7</v>
+      </c>
       <c r="L17" s="37"/>
       <c r="M17" s="36"/>
       <c r="N17" s="37"/>
@@ -2113,8 +2169,12 @@
       <c r="I18" s="19">
         <v>0.82</v>
       </c>
-      <c r="J18" s="37"/>
-      <c r="K18" s="36"/>
+      <c r="J18" s="17">
+        <v>0.62792697916666673</v>
+      </c>
+      <c r="K18" s="19">
+        <v>0.7</v>
+      </c>
       <c r="L18" s="37"/>
       <c r="M18" s="36"/>
       <c r="N18" s="37"/>
@@ -2159,8 +2219,12 @@
       <c r="I19" s="19">
         <v>0.82</v>
       </c>
-      <c r="J19" s="37"/>
-      <c r="K19" s="36"/>
+      <c r="J19" s="17">
+        <v>0.66964947916666662</v>
+      </c>
+      <c r="K19" s="19">
+        <v>0.72</v>
+      </c>
       <c r="L19" s="37"/>
       <c r="M19" s="36"/>
       <c r="N19" s="37"/>
@@ -2205,8 +2269,12 @@
       <c r="I20" s="19">
         <v>0.8</v>
       </c>
-      <c r="J20" s="37"/>
-      <c r="K20" s="36"/>
+      <c r="J20" s="17">
+        <v>0.71137166666666674</v>
+      </c>
+      <c r="K20" s="19">
+        <v>0.72</v>
+      </c>
       <c r="L20" s="37"/>
       <c r="M20" s="36"/>
       <c r="N20" s="37"/>
@@ -2251,8 +2319,12 @@
       <c r="I21" s="19">
         <v>0.81</v>
       </c>
-      <c r="J21" s="37"/>
-      <c r="K21" s="36"/>
+      <c r="J21" s="17">
+        <v>0.75309297453703705</v>
+      </c>
+      <c r="K21" s="19">
+        <v>0.71</v>
+      </c>
       <c r="L21" s="37"/>
       <c r="M21" s="36"/>
       <c r="N21" s="37"/>
@@ -2297,8 +2369,12 @@
       <c r="I22" s="19">
         <v>0.77</v>
       </c>
-      <c r="J22" s="37"/>
-      <c r="K22" s="36"/>
+      <c r="J22" s="17">
+        <v>0.79481415509259257</v>
+      </c>
+      <c r="K22" s="19">
+        <v>0.7</v>
+      </c>
       <c r="L22" s="37"/>
       <c r="M22" s="36"/>
       <c r="N22" s="37"/>
@@ -2340,11 +2416,15 @@
       <c r="H23" s="17">
         <v>0.8352278125</v>
       </c>
-      <c r="I23" s="58">
+      <c r="I23" s="40">
         <v>0.37</v>
       </c>
-      <c r="J23" s="37"/>
-      <c r="K23" s="36"/>
+      <c r="J23" s="17">
+        <v>0.83653473379629628</v>
+      </c>
+      <c r="K23" s="19">
+        <v>0.7</v>
+      </c>
       <c r="L23" s="37"/>
       <c r="M23" s="36"/>
       <c r="N23" s="37"/>
@@ -2389,8 +2469,12 @@
       <c r="I24" s="19">
         <v>0.7</v>
       </c>
-      <c r="J24" s="37"/>
-      <c r="K24" s="36"/>
+      <c r="J24" s="17">
+        <v>0.87825468750000002</v>
+      </c>
+      <c r="K24" s="19">
+        <v>0.73</v>
+      </c>
       <c r="L24" s="37"/>
       <c r="M24" s="36"/>
       <c r="N24" s="37"/>
@@ -2435,8 +2519,12 @@
       <c r="I25" s="19">
         <v>0.71</v>
       </c>
-      <c r="J25" s="37"/>
-      <c r="K25" s="36"/>
+      <c r="J25" s="17">
+        <v>0.91997454861111116</v>
+      </c>
+      <c r="K25" s="19">
+        <v>0.73</v>
+      </c>
       <c r="L25" s="37"/>
       <c r="M25" s="36"/>
       <c r="N25" s="37"/>
@@ -2481,8 +2569,12 @@
       <c r="I26" s="19">
         <v>0.73</v>
       </c>
-      <c r="J26" s="37"/>
-      <c r="K26" s="36"/>
+      <c r="J26" s="17">
+        <v>0.96169420138888895</v>
+      </c>
+      <c r="K26" s="19">
+        <v>0.69</v>
+      </c>
       <c r="L26" s="37"/>
       <c r="M26" s="36"/>
       <c r="N26" s="37"/>
@@ -2527,8 +2619,12 @@
       <c r="I27" s="19">
         <v>0.75</v>
       </c>
-      <c r="J27" s="37"/>
-      <c r="K27" s="36"/>
+      <c r="J27" s="17">
+        <v>3.4136921296296294E-3</v>
+      </c>
+      <c r="K27" s="19">
+        <v>0.74</v>
+      </c>
       <c r="L27" s="37"/>
       <c r="M27" s="36"/>
       <c r="N27" s="37"/>
@@ -2579,9 +2675,9 @@
       <c r="J28" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="K28" s="38" t="e">
+      <c r="K28" s="39">
         <f t="shared" ref="K28" si="0">AVERAGE(K4:K27)</f>
-        <v>#DIV/0!</v>
+        <v>0.72375</v>
       </c>
       <c r="L28" s="6" t="s">
         <v>2</v>
@@ -2697,66 +2793,66 @@
       <c r="E30" s="19">
         <v>0.79</v>
       </c>
-      <c r="F30" s="49" t="s">
+      <c r="F30" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="G30" s="50"/>
-      <c r="H30" s="49" t="s">
+      <c r="G30" s="56"/>
+      <c r="H30" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="I30" s="55"/>
-      <c r="J30" s="49" t="s">
+      <c r="I30" s="44"/>
+      <c r="J30" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="K30" s="55"/>
-      <c r="L30" s="49" t="s">
+      <c r="K30" s="44"/>
+      <c r="L30" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="M30" s="55"/>
-      <c r="N30" s="49" t="s">
+      <c r="M30" s="44"/>
+      <c r="N30" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="O30" s="55"/>
-      <c r="P30" s="49" t="s">
+      <c r="O30" s="44"/>
+      <c r="P30" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="Q30" s="55"/>
-      <c r="R30" s="49" t="s">
+      <c r="Q30" s="44"/>
+      <c r="R30" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="S30" s="55"/>
-      <c r="T30" s="49" t="s">
+      <c r="S30" s="44"/>
+      <c r="T30" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="U30" s="55"/>
-      <c r="V30" s="49" t="s">
+      <c r="U30" s="44"/>
+      <c r="V30" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="W30" s="55"/>
-      <c r="X30" s="49" t="s">
+      <c r="W30" s="44"/>
+      <c r="X30" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="Y30" s="55"/>
-      <c r="Z30" s="49" t="s">
+      <c r="Y30" s="44"/>
+      <c r="Z30" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="AA30" s="55"/>
-      <c r="AB30" s="49" t="s">
+      <c r="AA30" s="44"/>
+      <c r="AB30" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="AC30" s="55"/>
-      <c r="AD30" s="49" t="s">
+      <c r="AC30" s="44"/>
+      <c r="AD30" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="AE30" s="55"/>
-      <c r="AF30" s="49" t="s">
+      <c r="AE30" s="44"/>
+      <c r="AF30" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="AG30" s="55"/>
-      <c r="AH30" s="49" t="s">
+      <c r="AG30" s="44"/>
+      <c r="AH30" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="AI30" s="55"/>
+      <c r="AI30" s="44"/>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
@@ -3287,138 +3383,138 @@
       <c r="E38" s="19">
         <v>0.76</v>
       </c>
-      <c r="F38" s="51" t="s">
+      <c r="F38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="G38" s="52"/>
-      <c r="H38" s="51" t="s">
+      <c r="G38" s="57"/>
+      <c r="H38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="I38" s="56"/>
-      <c r="J38" s="51" t="s">
+      <c r="I38" s="42"/>
+      <c r="J38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="K38" s="56"/>
-      <c r="L38" s="51" t="s">
+      <c r="K38" s="42"/>
+      <c r="L38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="M38" s="56"/>
-      <c r="N38" s="51" t="s">
+      <c r="M38" s="42"/>
+      <c r="N38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="O38" s="56"/>
-      <c r="P38" s="51" t="s">
+      <c r="O38" s="42"/>
+      <c r="P38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="Q38" s="56"/>
-      <c r="R38" s="51" t="s">
+      <c r="Q38" s="42"/>
+      <c r="R38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="S38" s="56"/>
-      <c r="T38" s="51" t="s">
+      <c r="S38" s="42"/>
+      <c r="T38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="U38" s="56"/>
-      <c r="V38" s="51" t="s">
+      <c r="U38" s="42"/>
+      <c r="V38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="W38" s="56"/>
-      <c r="X38" s="51" t="s">
+      <c r="W38" s="42"/>
+      <c r="X38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="Y38" s="56"/>
-      <c r="Z38" s="51" t="s">
+      <c r="Y38" s="42"/>
+      <c r="Z38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="AA38" s="56"/>
-      <c r="AB38" s="51" t="s">
+      <c r="AA38" s="42"/>
+      <c r="AB38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="AC38" s="56"/>
-      <c r="AD38" s="51" t="s">
+      <c r="AC38" s="42"/>
+      <c r="AD38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="AE38" s="56"/>
-      <c r="AF38" s="51" t="s">
+      <c r="AE38" s="42"/>
+      <c r="AF38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="AG38" s="56"/>
-      <c r="AH38" s="51" t="s">
+      <c r="AG38" s="42"/>
+      <c r="AH38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="AI38" s="56"/>
+      <c r="AI38" s="42"/>
     </row>
     <row r="39" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="46" t="s">
+      <c r="B39" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="C39" s="47"/>
+      <c r="C39" s="52"/>
       <c r="D39" s="17">
         <v>0.36553122685185185</v>
       </c>
       <c r="E39" s="19">
         <v>0.75</v>
       </c>
-      <c r="F39" s="53" t="s">
+      <c r="F39" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="G39" s="54"/>
-      <c r="H39" s="53" t="s">
+      <c r="G39" s="58"/>
+      <c r="H39" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="I39" s="57"/>
-      <c r="J39" s="53" t="s">
+      <c r="I39" s="46"/>
+      <c r="J39" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="K39" s="57"/>
-      <c r="L39" s="53" t="s">
+      <c r="K39" s="46"/>
+      <c r="L39" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="M39" s="57"/>
-      <c r="N39" s="53" t="s">
+      <c r="M39" s="46"/>
+      <c r="N39" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="O39" s="57"/>
-      <c r="P39" s="53" t="s">
+      <c r="O39" s="46"/>
+      <c r="P39" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="Q39" s="57"/>
-      <c r="R39" s="53" t="s">
+      <c r="Q39" s="46"/>
+      <c r="R39" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="S39" s="57"/>
-      <c r="T39" s="53" t="s">
+      <c r="S39" s="46"/>
+      <c r="T39" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="U39" s="57"/>
-      <c r="V39" s="53" t="s">
+      <c r="U39" s="46"/>
+      <c r="V39" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="W39" s="57"/>
-      <c r="X39" s="53" t="s">
+      <c r="W39" s="46"/>
+      <c r="X39" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="Y39" s="57"/>
-      <c r="Z39" s="53" t="s">
+      <c r="Y39" s="46"/>
+      <c r="Z39" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="AA39" s="57"/>
-      <c r="AB39" s="53" t="s">
+      <c r="AA39" s="46"/>
+      <c r="AB39" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="AC39" s="57"/>
-      <c r="AD39" s="53" t="s">
+      <c r="AC39" s="46"/>
+      <c r="AD39" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="AE39" s="57"/>
-      <c r="AF39" s="53" t="s">
+      <c r="AE39" s="46"/>
+      <c r="AF39" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="AG39" s="57"/>
-      <c r="AH39" s="53" t="s">
+      <c r="AG39" s="46"/>
+      <c r="AH39" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="AI39" s="57"/>
+      <c r="AI39" s="46"/>
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
@@ -3521,10 +3617,10 @@
       <c r="G46" s="28"/>
     </row>
     <row r="47" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B47" s="42" t="s">
+      <c r="B47" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C47" s="43"/>
+      <c r="C47" s="48"/>
       <c r="D47" s="17">
         <v>0.44897613425925925</v>
       </c>
@@ -3535,10 +3631,10 @@
       <c r="G47" s="28"/>
     </row>
     <row r="48" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="44" t="s">
+      <c r="B48" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="C48" s="45"/>
+      <c r="C48" s="50"/>
       <c r="D48" s="17">
         <v>0.4594068634259259</v>
       </c>
@@ -3911,10 +4007,10 @@
       <c r="D94" s="1"/>
     </row>
     <row r="95" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D95" s="49" t="s">
+      <c r="D95" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E95" s="55"/>
+      <c r="E95" s="44"/>
     </row>
     <row r="96" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D96" s="4" t="s">
@@ -3959,19 +4055,71 @@
     </row>
     <row r="102" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="103" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D103" s="51" t="s">
+      <c r="D103" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="E103" s="56"/>
+      <c r="E103" s="42"/>
     </row>
     <row r="104" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D104" s="53" t="s">
+      <c r="D104" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="E104" s="57"/>
+      <c r="E104" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="68">
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="R30:S30"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="X30:Y30"/>
+    <mergeCell ref="Z30:AA30"/>
+    <mergeCell ref="T38:U38"/>
+    <mergeCell ref="V38:W38"/>
+    <mergeCell ref="X38:Y38"/>
+    <mergeCell ref="Z38:AA38"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="R38:S38"/>
+    <mergeCell ref="AH39:AI39"/>
+    <mergeCell ref="AB30:AC30"/>
+    <mergeCell ref="AD30:AE30"/>
+    <mergeCell ref="AF30:AG30"/>
+    <mergeCell ref="AH30:AI30"/>
+    <mergeCell ref="AD38:AE38"/>
+    <mergeCell ref="AF38:AG38"/>
+    <mergeCell ref="AB38:AC38"/>
     <mergeCell ref="D103:E103"/>
     <mergeCell ref="D95:E95"/>
     <mergeCell ref="D104:E104"/>
@@ -3988,58 +4136,6 @@
     <mergeCell ref="AB39:AC39"/>
     <mergeCell ref="AD39:AE39"/>
     <mergeCell ref="AF39:AG39"/>
-    <mergeCell ref="AH39:AI39"/>
-    <mergeCell ref="AB30:AC30"/>
-    <mergeCell ref="AD30:AE30"/>
-    <mergeCell ref="AF30:AG30"/>
-    <mergeCell ref="AH30:AI30"/>
-    <mergeCell ref="AD38:AE38"/>
-    <mergeCell ref="AF38:AG38"/>
-    <mergeCell ref="AB38:AC38"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="L38:M38"/>
-    <mergeCell ref="N38:O38"/>
-    <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="R38:S38"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="X30:Y30"/>
-    <mergeCell ref="Z30:AA30"/>
-    <mergeCell ref="T38:U38"/>
-    <mergeCell ref="V38:W38"/>
-    <mergeCell ref="X38:Y38"/>
-    <mergeCell ref="Z38:AA38"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="R30:S30"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>